<commit_message>
* Fixed in-IRQ freezing bug (USE_FPU added)
</commit_message>
<xml_diff>
--- a/Microom_hw/BOM.xlsx
+++ b/Microom_hw/BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11550"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="90">
   <si>
     <t>Reference</t>
   </si>
@@ -287,9 +287,6 @@
   </si>
   <si>
     <t>Availability</t>
-  </si>
-  <si>
-    <t>Надо добыть</t>
   </si>
   <si>
     <t>Есть</t>
@@ -324,9 +321,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;₽&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;₽&quot;"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -346,14 +343,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -402,7 +391,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -412,11 +401,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
     <fill>
@@ -484,44 +468,41 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="7"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="6" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="5" fillId="5" borderId="1" xfId="4" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="5"/>
-    <xf numFmtId="165" fontId="6" fillId="6" borderId="1" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4"/>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="4" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="8">
-    <cellStyle name="Accent1" xfId="7" builtinId="29"/>
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Calculation" xfId="5" builtinId="22"/>
+  <cellStyles count="7">
+    <cellStyle name="Accent1" xfId="6" builtinId="29"/>
+    <cellStyle name="Calculation" xfId="4" builtinId="22"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Input" xfId="4" builtinId="20"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
+    <cellStyle name="Input" xfId="3" builtinId="20"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="6" builtinId="10"/>
+    <cellStyle name="Note" xfId="5" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -806,7 +787,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="F15" sqref="F14:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,10 +820,10 @@
         <v>80</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -858,13 +839,13 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="G2" s="9">
+      <c r="F2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" s="8">
         <v>5</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="8">
         <f>B2*G2</f>
         <v>65</v>
       </c>
@@ -883,12 +864,12 @@
         <v>10</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G3" s="9">
+        <v>81</v>
+      </c>
+      <c r="G3" s="8">
         <v>3</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="8">
         <f t="shared" ref="H3:H25" si="0">B3*G3</f>
         <v>21</v>
       </c>
@@ -907,12 +888,12 @@
         <v>10</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G4" s="9">
+        <v>81</v>
+      </c>
+      <c r="G4" s="8">
         <v>3</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="8">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
@@ -931,12 +912,12 @@
         <v>10</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G5" s="9">
+        <v>81</v>
+      </c>
+      <c r="G5" s="8">
         <v>1</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="8">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -955,12 +936,12 @@
         <v>10</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G6" s="9">
+        <v>81</v>
+      </c>
+      <c r="G6" s="8">
         <v>1</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="8">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -979,12 +960,12 @@
         <v>10</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G7" s="9">
+        <v>81</v>
+      </c>
+      <c r="G7" s="8">
         <v>1</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="8">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -1002,13 +983,13 @@
       <c r="D8" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G8" s="9">
+      <c r="F8" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G8" s="8">
         <v>24</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="8">
         <f t="shared" si="0"/>
         <v>216</v>
       </c>
@@ -1029,13 +1010,13 @@
       <c r="E9" t="s">
         <v>73</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G9" s="9">
+      <c r="F9" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G9" s="8">
         <v>25</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="8">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
@@ -1056,11 +1037,11 @@
       <c r="E10" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10">
+      <c r="F10" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1081,13 +1062,13 @@
       <c r="E11" t="s">
         <v>75</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G11" s="9">
+      <c r="F11" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G11" s="8">
         <v>770</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="8">
         <f t="shared" si="0"/>
         <v>770</v>
       </c>
@@ -1109,12 +1090,12 @@
         <v>78</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G12" s="9">
+        <v>81</v>
+      </c>
+      <c r="G12" s="8">
         <v>0.5</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="8">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1133,10 +1114,10 @@
         <v>42</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10">
+        <v>83</v>
+      </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1157,13 +1138,13 @@
       <c r="E14" t="s">
         <v>79</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="G14" s="9">
+      <c r="F14" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" s="8">
         <v>80.5</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="8">
         <f t="shared" si="0"/>
         <v>80.5</v>
       </c>
@@ -1182,12 +1163,12 @@
         <v>48</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G15" s="9">
+        <v>81</v>
+      </c>
+      <c r="G15" s="8">
         <v>0.5</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="8">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
@@ -1206,12 +1187,12 @@
         <v>48</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G16" s="9">
+        <v>81</v>
+      </c>
+      <c r="G16" s="8">
         <v>0.5</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H16" s="8">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -1230,12 +1211,12 @@
         <v>48</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G17" s="9">
+        <v>81</v>
+      </c>
+      <c r="G17" s="8">
         <v>0.5</v>
       </c>
-      <c r="H17" s="9">
+      <c r="H17" s="8">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
@@ -1254,12 +1235,12 @@
         <v>48</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="G18" s="9">
+        <v>84</v>
+      </c>
+      <c r="G18" s="8">
         <v>0.5</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="8">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -1278,12 +1259,12 @@
         <v>48</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G19" s="9">
+        <v>81</v>
+      </c>
+      <c r="G19" s="8">
         <v>0.5</v>
       </c>
-      <c r="H19" s="9">
+      <c r="H19" s="8">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -1295,19 +1276,19 @@
       <c r="B20">
         <v>9</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="7">
         <v>510</v>
       </c>
       <c r="D20" t="s">
         <v>48</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G20" s="9">
+        <v>81</v>
+      </c>
+      <c r="G20" s="8">
         <v>0.5</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="8">
         <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
@@ -1326,12 +1307,12 @@
         <v>63</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G21" s="9">
+        <v>81</v>
+      </c>
+      <c r="G21" s="8">
         <v>3</v>
       </c>
-      <c r="H21" s="9">
+      <c r="H21" s="8">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -1350,12 +1331,12 @@
         <v>66</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G22" s="9">
+        <v>81</v>
+      </c>
+      <c r="G22" s="8">
         <v>40</v>
       </c>
-      <c r="H22" s="9">
+      <c r="H22" s="8">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
@@ -1374,12 +1355,12 @@
         <v>69</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G23" s="9">
+        <v>81</v>
+      </c>
+      <c r="G23" s="8">
         <v>4</v>
       </c>
-      <c r="H23" s="9">
+      <c r="H23" s="8">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -1398,42 +1379,42 @@
         <v>72</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G24" s="9">
+        <v>81</v>
+      </c>
+      <c r="G24" s="8">
         <v>40</v>
       </c>
-      <c r="H24" s="9">
+      <c r="H24" s="8">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G25" s="10">
+        <v>82</v>
+      </c>
+      <c r="G25" s="9">
         <v>1250</v>
       </c>
-      <c r="H25" s="10">
+      <c r="H25" s="9">
         <f t="shared" si="0"/>
         <v>1250</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G26" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="H26" s="12">
+      <c r="G26" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="H26" s="11">
         <f>SUM(H2:H25)</f>
         <v>2601</v>
       </c>

</xml_diff>